<commit_message>
updated swal and questions
</commit_message>
<xml_diff>
--- a/src/questions.xlsx
+++ b/src/questions.xlsx
@@ -1,33 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rileycammack/Desktop/covid project/react-tictactoe/react-tictactoe/src/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="6480" yWindow="4420" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
-  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+  <si>
+    <t>who would they push off a cliff</t>
+  </si>
+  <si>
+    <t>who would push them off a cliff</t>
+  </si>
+  <si>
+    <t>what would they get a tattoo of</t>
+  </si>
   <si>
     <t>how do they 'really' spend their weekends</t>
   </si>
@@ -35,15 +28,6 @@
     <t>if they were on a date from hell, how would they get out of it</t>
   </si>
   <si>
-    <t>what would they get a tattoo of</t>
-  </si>
-  <si>
-    <t>who would they push off a cliff</t>
-  </si>
-  <si>
-    <t>who would push them off a cliff</t>
-  </si>
-  <si>
     <t>what are they terrible at</t>
   </si>
   <si>
@@ -147,186 +131,224 @@
   </si>
   <si>
     <t>if they won one million dollars, what would they buy first</t>
+  </si>
+  <si>
+    <t>if they were on a deserted island, what would they take with them</t>
+  </si>
+  <si>
+    <t>what is one class they would love to take</t>
+  </si>
+  <si>
+    <t>what one possession are they embarassed to have</t>
+  </si>
+  <si>
+    <t>if they were invisible where would they go</t>
+  </si>
+  <si>
+    <t>if they were in an olympic sport what would it be</t>
+  </si>
+  <si>
+    <t>if they were an expert in one subject, what would it be</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if they had a super power what would it be </t>
+  </si>
+  <si>
+    <t>if they owned a yacht, what would they name it</t>
+  </si>
+  <si>
+    <t>what 3 words come to mind when you think of them</t>
+  </si>
+  <si>
+    <t>if they could add a feature to their phone what would it be</t>
+  </si>
+  <si>
+    <t>what would they put on their ice cream</t>
+  </si>
+  <si>
+    <t>what is their favorite time of day</t>
+  </si>
+  <si>
+    <t>where is their ideal place to live</t>
+  </si>
+  <si>
+    <t>if they could live in any era, which would it be</t>
+  </si>
+  <si>
+    <t>what store would they never be caught dead in</t>
+  </si>
+  <si>
+    <t>what is their ideal location to be proposed to</t>
+  </si>
+  <si>
+    <t>if someone wrote a book about them, what would the title be</t>
+  </si>
+  <si>
+    <t xml:space="preserve">who would play them in a movie </t>
+  </si>
+  <si>
+    <t>what do they need more of in their life</t>
+  </si>
+  <si>
+    <t>what would make them happy right now</t>
+  </si>
+  <si>
+    <t>if they could share one thing with the world, what would it be</t>
+  </si>
+  <si>
+    <t>what do they love about themselves</t>
+  </si>
+  <si>
+    <t>what advice would they give to their younger self</t>
+  </si>
+  <si>
+    <t>what does their ideal morning look like</t>
+  </si>
+  <si>
+    <t>when was the last time they truly felt alive</t>
+  </si>
+  <si>
+    <t>what is something they would love to learn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what can they do to better take care of themselves </t>
+  </si>
+  <si>
+    <t>what do they want their legacy to be</t>
+  </si>
+  <si>
+    <t>what will be written on their tombstone</t>
+  </si>
+  <si>
+    <t>what is something that offends them</t>
+  </si>
+  <si>
+    <t>how do they recharge</t>
+  </si>
+  <si>
+    <t>what is their favorite food</t>
+  </si>
+  <si>
+    <t>what do they always forget</t>
+  </si>
+  <si>
+    <t>what is their favorite outdoor activity</t>
+  </si>
+  <si>
+    <t>what do they hate more than anything</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="4">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+  <cellXfs count="4">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Sheets">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4285F4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="EA4335"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="FBBC04"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="34A853"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="FF6D01"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="46BDC6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="1155CC"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="1155CC"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -467,238 +489,398 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="86" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="44.1640625" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="92.14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" ht="74" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" ht="77" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24">
+      <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="27">
+      <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="28">
+      <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29">
+      <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30">
+      <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31">
+      <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32">
+      <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="33">
+      <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="34">
+      <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="35">
+      <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="36">
+      <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="37">
+      <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="38">
+      <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="39">
+      <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="40">
+      <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>